<commit_message>
[TISNEW-370] Logic to implement create assessment, refactoring the hardcoded values to actual values
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/TIS Assessment Import Template - Step 2.xlsx
+++ b/generic-upload-service/src/test/resources/TIS Assessment Import Template - Step 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunil/dev/TIS/TIS-GENERIC-UPLOAD/generic-upload-service/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D59243DC-9D58-AC4C-8052-A92F9099B6E4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{813C65C9-F56A-BF41-8940-F1F737B0B808}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="8900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Review date*</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Period covered from</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>Responsible officer comments is to blah blah blah.</t>
+  </si>
+  <si>
+    <t>Type*</t>
   </si>
 </sst>
 </file>
@@ -225,7 +225,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -299,7 +299,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +584,7 @@
   <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -640,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
@@ -658,16 +658,16 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>14</v>
@@ -724,7 +724,7 @@
         <v>25</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>17</v>
@@ -733,12 +733,12 @@
         <v>18</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>8000600</v>
@@ -746,22 +746,22 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" t="s">
-        <v>43</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I2" s="11">
         <v>43678</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="6">
         <v>43647</v>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>8000601</v>
@@ -795,19 +795,19 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I3" s="11">
         <v>43678</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K3" s="6">
         <v>43647</v>
@@ -825,18 +825,18 @@
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="S3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3">
         <v>8000603</v>
@@ -844,19 +844,19 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="I4" s="11">
         <v>43678</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="6">
         <v>43647</v>
@@ -874,21 +874,21 @@
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q4">
         <v>3</v>
       </c>
       <c r="S4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" t="s">
         <v>49</v>
-      </c>
-      <c r="T4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>8000604</v>
@@ -896,22 +896,22 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
       <c r="G5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I5" s="11">
         <v>45505</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="6">
         <v>45474</v>
@@ -929,15 +929,15 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>8000605</v>
@@ -945,22 +945,22 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
         <v>42</v>
       </c>
-      <c r="F6" t="s">
-        <v>43</v>
-      </c>
       <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I6" s="11">
         <v>45505</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K6" s="6">
         <v>45474</v>
@@ -978,15 +978,15 @@
         <v>5</v>
       </c>
       <c r="P6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" t="s">
         <v>46</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>8000606</v>
@@ -994,22 +994,22 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
       <c r="G7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="11">
+        <v>45505</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="I7" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="K7" s="6">
         <v>45474</v>
@@ -1027,66 +1027,66 @@
         <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q7">
         <v>1</v>
       </c>
       <c r="R7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U7" t="s">
+        <v>51</v>
+      </c>
+      <c r="V7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W7" t="s">
         <v>52</v>
       </c>
-      <c r="V7" t="s">
-        <v>44</v>
-      </c>
-      <c r="W7" t="s">
-        <v>53</v>
-      </c>
       <c r="X7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y7" s="6">
         <v>42186</v>
       </c>
       <c r="Z7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AA7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AF7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AH7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AH7" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AJ7" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="AJ7" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3">
         <v>8000607</v>
@@ -1094,22 +1094,22 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
       <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I8" s="11">
         <v>45505</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K8" s="6">
         <v>45474</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1137,22 +1137,22 @@
         <v>8000608</v>
       </c>
       <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
       <c r="G9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I9" s="11">
         <v>45505</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="6">
         <v>45474</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1180,22 +1180,22 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
         <v>42</v>
       </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
       <c r="G10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I10" s="11">
         <v>45505</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="6">
         <v>45474</v>
@@ -1215,30 +1215,30 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="I11" s="11">
         <v>45505</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K11" s="6">
         <v>45474</v>

</xml_diff>

<commit_message>
Update the test templates
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/TIS Assessment Import Template - Step 2.xlsx
+++ b/generic-upload-service/src/test/resources/TIS Assessment Import Template - Step 2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunil/dev/TIS/TIS-GENERIC-UPLOAD/generic-upload-service/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yafang.deng\Documents\git\TIS-GENERIC-UPLOAD\generic-upload-service\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{813C65C9-F56A-BF41-8940-F1F737B0B808}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C052E8F-C31A-447F-9D1E-24296EB14C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="8900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIS Assessment template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIS Assessment template'!$A$1:$AJ$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TIS Assessment template'!$A$1:$AG$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="59">
   <si>
     <t>Trainee Surname*</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Curriculum name*</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Outcome</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>10% audit - lay member</t>
   </si>
   <si>
-    <t>Trainee notified of outcome</t>
-  </si>
-  <si>
     <t>Review date*</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>Responsible officer comments</t>
   </si>
   <si>
-    <t>Portfolio review date</t>
-  </si>
-  <si>
     <t>Ransoo</t>
   </si>
   <si>
@@ -154,9 +145,6 @@
   </si>
   <si>
     <t>ARCP</t>
-  </si>
-  <si>
-    <t>SCHEDULED</t>
   </si>
   <si>
     <t>YES</t>
@@ -581,52 +569,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AG14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="57.5" customWidth="1"/>
-    <col min="27" max="27" width="21" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="44.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="57.453125" customWidth="1"/>
+    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -640,105 +626,96 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>8000600</v>
@@ -746,48 +723,42 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="11">
+        <v>35</v>
+      </c>
+      <c r="H2" s="11">
         <v>43678</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>43313</v>
+      </c>
+      <c r="L2" s="6">
+        <v>43678</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>39</v>
-      </c>
-      <c r="K2" s="6">
-        <v>43647</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="6">
-        <v>43313</v>
-      </c>
-      <c r="N2" s="6">
-        <v>43678</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3">
         <v>8000601</v>
@@ -795,48 +766,45 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="11">
+        <v>35</v>
+      </c>
+      <c r="H3" s="11">
         <v>43678</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6">
+        <v>43313</v>
+      </c>
+      <c r="L3" s="6">
+        <v>43678</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3" t="s">
         <v>39</v>
-      </c>
-      <c r="K3" s="6">
-        <v>43647</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3" s="6">
-        <v>43313</v>
-      </c>
-      <c r="N3" s="6">
-        <v>43678</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>43</v>
       </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="S3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>8000603</v>
@@ -844,51 +812,48 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="11">
+        <v>35</v>
+      </c>
+      <c r="H4" s="11">
         <v>43678</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" s="6">
+        <v>43313</v>
+      </c>
+      <c r="L4" s="6">
+        <v>43678</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
         <v>39</v>
-      </c>
-      <c r="K4" s="6">
-        <v>43647</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-      <c r="M4" s="6">
-        <v>43313</v>
-      </c>
-      <c r="N4" s="6">
-        <v>43678</v>
       </c>
       <c r="O4">
         <v>3</v>
       </c>
-      <c r="P4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
-        <v>48</v>
-      </c>
-      <c r="T4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="Q4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>8000604</v>
@@ -896,48 +861,42 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" s="6">
+        <v>45139</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-      <c r="M5" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N5" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="O5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="3">
         <v>8000605</v>
@@ -945,48 +904,42 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" s="6">
+        <v>45139</v>
+      </c>
+      <c r="L6" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
+      <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L6">
-        <v>5</v>
-      </c>
-      <c r="M6" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N6" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O6">
-        <v>5</v>
-      </c>
-      <c r="P6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" ht="60" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:33" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" s="3">
         <v>8000606</v>
@@ -994,99 +947,90 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7" s="6">
+        <v>45139</v>
+      </c>
+      <c r="L7" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-      <c r="M7" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N7" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O7">
-        <v>6</v>
-      </c>
-      <c r="P7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>43</v>
+      <c r="S7" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" t="s">
+        <v>39</v>
       </c>
       <c r="U7" t="s">
+        <v>48</v>
+      </c>
+      <c r="V7" s="6">
+        <v>42186</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="V7" t="s">
-        <v>43</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="AA7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="X7" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y7" s="6">
-        <v>42186</v>
-      </c>
-      <c r="Z7" s="8" t="s">
+      <c r="AB7" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AA7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AC7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AE7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AG7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AF7" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG7" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH7" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ7" s="8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3">
         <v>8000607</v>
@@ -1094,42 +1038,36 @@
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>40</v>
+      <c r="J8">
+        <v>7</v>
       </c>
       <c r="K8" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L8">
+        <v>45139</v>
+      </c>
+      <c r="L8" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="M8" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N8" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1137,42 +1075,36 @@
         <v>8000608</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>40</v>
+      <c r="J9">
+        <v>8</v>
       </c>
       <c r="K9" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L9">
+        <v>45139</v>
+      </c>
+      <c r="L9" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M9">
         <v>8</v>
       </c>
-      <c r="M9" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N9" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3">
@@ -1180,93 +1112,81 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>40</v>
+      <c r="J10">
+        <v>9</v>
       </c>
       <c r="K10" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L10">
+        <v>45139</v>
+      </c>
+      <c r="L10" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M10">
         <v>9</v>
       </c>
-      <c r="M10" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N10" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="11">
+        <v>45505</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="11">
-        <v>45505</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>40</v>
+      <c r="J11">
+        <v>10</v>
       </c>
       <c r="K11" s="6">
-        <v>45474</v>
-      </c>
-      <c r="L11">
+        <v>45139</v>
+      </c>
+      <c r="L11" s="6">
+        <v>45505</v>
+      </c>
+      <c r="M11">
         <v>10</v>
       </c>
-      <c r="M11" s="6">
-        <v>45139</v>
-      </c>
-      <c r="N11" s="6">
-        <v>45505</v>
-      </c>
-      <c r="O11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>

</xml_diff>